<commit_message>
Add van de dag
</commit_message>
<xml_diff>
--- a/Documentatie Fifa/Fase 1/Logboek.xlsx
+++ b/Documentatie Fifa/Fase 1/Logboek.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dion Rodie\Desktop\Radius\Projects\Csharpfifa\FifaCsharp\Documentatie Fifa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dion Rodie\Desktop\Radius\Projects\Csharpfifa\FifaCsharp\Documentatie Fifa\Fase 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Datum</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Tim heeft moeite met mee komen</t>
+  </si>
+  <si>
+    <t>Iedereen heeft goed gewerkt</t>
   </si>
 </sst>
 </file>
@@ -444,7 +447,7 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -505,7 +508,21 @@
       <c r="A4" s="3">
         <v>42844</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
@@ -729,19 +746,19 @@
       <c r="A47" s="3"/>
       <c r="B47" s="4">
         <f>SUM(B3:B44)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C47">
         <f>SUM(C3:C44)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D47">
         <f>SUM(D3:D44)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E47">
         <f>SUM(E3:E44)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -752,7 +769,7 @@
     <row r="50" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <f>SUM(B47:E47)</f>
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>